<commit_message>
Update test to have tmp as dir
</commit_message>
<xml_diff>
--- a/tests/data/test_data_01.xlsx
+++ b/tests/data/test_data_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042D154A-4E9A-C347-8CB9-76D641964D7C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA9129D-041C-E249-B1FC-B1D633BDFC19}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
     <t>MONEY</t>
   </si>
   <si>
-    <t>nlp/test_data_01</t>
+    <t>[tmp]/nlp/test_data_01</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Refactor test Remove ner check
</commit_message>
<xml_diff>
--- a/tests/data/test_data_01.xlsx
+++ b/tests/data/test_data_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA9129D-041C-E249-B1FC-B1D633BDFC19}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE308361-0D77-4C4A-AD66-8E8FAF54D1BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -422,7 +422,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D581B7A-DDFF-5C48-A6CD-60228BBE6862}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Update test Reduce iteration Update travis config
</commit_message>
<xml_diff>
--- a/tests/data/test_data_01.xlsx
+++ b/tests/data/test_data_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE308361-0D77-4C4A-AD66-8E8FAF54D1BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B78830D-0B39-A74E-B92D-C2989E50ECD8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -422,9 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D581B7A-DDFF-5C48-A6CD-60228BBE6862}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -530,7 +528,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add new type of test data
</commit_message>
<xml_diff>
--- a/tests/data/test_data_01.xlsx
+++ b/tests/data/test_data_01.xlsx
@@ -8,20 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B78830D-0B39-A74E-B92D-C2989E50ECD8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00656A8F-C329-5A4C-9069-7FF168C9D304}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="train" sheetId="3" r:id="rId1"/>
-    <sheet name="config" sheetId="2" r:id="rId2"/>
+    <sheet name="source" sheetId="4" r:id="rId1"/>
+    <sheet name="prepare" sheetId="3" r:id="rId2"/>
+    <sheet name="train" sheetId="1" r:id="rId3"/>
+    <sheet name="config" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>subtext</t>
+  </si>
+  <si>
+    <t>span</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
   <si>
     <t>name</t>
   </si>
@@ -32,52 +49,121 @@
     <t>kind</t>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>base</t>
-  </si>
-  <si>
     <t>en_core_web_sm</t>
   </si>
   <si>
-    <t>train.iteration</t>
-  </si>
-  <si>
-    <t>train.drop</t>
-  </si>
-  <si>
-    <t>train.matcher</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>subtext</t>
-  </si>
-  <si>
-    <t>entity</t>
-  </si>
-  <si>
     <t>Uber blew through $1 million a week</t>
   </si>
   <si>
+    <t>Android Pay expands to Canada</t>
+  </si>
+  <si>
+    <t>Spotify steps up Asia expansion</t>
+  </si>
+  <si>
+    <t>Google Maps launches location sharing</t>
+  </si>
+  <si>
+    <t>Google rebrands its business apps</t>
+  </si>
+  <si>
+    <t>look what i found on google! 😂</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Google Maps</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
     <t>Uber</t>
   </si>
   <si>
+    <t>$1 million</t>
+  </si>
+  <si>
+    <t>MONEY</t>
+  </si>
+  <si>
+    <t>Spotify</t>
+  </si>
+  <si>
+    <t>Android Pay</t>
+  </si>
+  <si>
     <t>ORG</t>
   </si>
   <si>
-    <t>$1 million</t>
-  </si>
-  <si>
-    <t>MONEY</t>
-  </si>
-  <si>
-    <t>[tmp]/nlp/test_data_01</t>
+    <t>GPE</t>
+  </si>
+  <si>
+    <t>0,4</t>
+  </si>
+  <si>
+    <t>[tmp]/nlp/test_data_04</t>
+  </si>
+  <si>
+    <t>Uber blew through $1 million a week. Android Pay expands to Canada. Spotify steps up Asia expansion.</t>
+  </si>
+  <si>
+    <t>textract</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>regex</t>
+  </si>
+  <si>
+    <t>Uber?</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>phrase</t>
+  </si>
+  <si>
+    <t>nlp_name</t>
+  </si>
+  <si>
+    <t>nlp_base</t>
+  </si>
+  <si>
+    <t>train_iteration</t>
+  </si>
+  <si>
+    <t>train_drop</t>
+  </si>
+  <si>
+    <t>idx</t>
+  </si>
+  <si>
+    <t>prepare_enabled</t>
+  </si>
+  <si>
+    <t>source_language</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>source/test_source_01.txt</t>
   </si>
 </sst>
 </file>
@@ -419,29 +505,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D581B7A-DDFF-5C48-A6CD-60228BBE6862}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BF5D81-E310-3A45-9ABE-A86114765ABD}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="3" max="3" width="78.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B93662-D338-7A4C-897B-C0C87D585A42}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -449,37 +586,239 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1.1000000000000001</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1.2</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1.2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2.1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3.1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3.2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>6.1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -487,64 +826,64 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1">
-        <v>0.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="b">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor span to string Add train logic Add config
</commit_message>
<xml_diff>
--- a/tests/data/test_data_01.xlsx
+++ b/tests/data/test_data_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00656A8F-C329-5A4C-9069-7FF168C9D304}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590E407B-9734-5B48-A43D-EBA8F9020C61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>text</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>source/test_source_01.txt</t>
+  </si>
+  <si>
+    <t>train_autosave</t>
   </si>
 </sst>
 </file>
@@ -633,7 +636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="C6:E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -820,7 +825,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -886,6 +891,14 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix bug in prepare pipe Refactor to support nlp load from base Update data set Update README
</commit_message>
<xml_diff>
--- a/tests/data/test_data_01.xlsx
+++ b/tests/data/test_data_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590E407B-9734-5B48-A43D-EBA8F9020C61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6392AE28-F5DC-654B-85F2-5C10B79E8EC2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>text</t>
   </si>
@@ -52,69 +52,15 @@
     <t>en_core_web_sm</t>
   </si>
   <si>
-    <t>Uber blew through $1 million a week</t>
-  </si>
-  <si>
-    <t>Android Pay expands to Canada</t>
-  </si>
-  <si>
-    <t>Spotify steps up Asia expansion</t>
-  </si>
-  <si>
-    <t>Google Maps launches location sharing</t>
-  </si>
-  <si>
-    <t>Google rebrands its business apps</t>
-  </si>
-  <si>
-    <t>look what i found on google! 😂</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>LOC</t>
-  </si>
-  <si>
-    <t>Asia</t>
-  </si>
-  <si>
-    <t>Google Maps</t>
-  </si>
-  <si>
     <t>PRODUCT</t>
   </si>
   <si>
-    <t>Google</t>
-  </si>
-  <si>
     <t>google</t>
   </si>
   <si>
-    <t>Uber</t>
-  </si>
-  <si>
-    <t>$1 million</t>
-  </si>
-  <si>
-    <t>MONEY</t>
-  </si>
-  <si>
-    <t>Spotify</t>
-  </si>
-  <si>
-    <t>Android Pay</t>
-  </si>
-  <si>
     <t>ORG</t>
   </si>
   <si>
-    <t>GPE</t>
-  </si>
-  <si>
-    <t>0,4</t>
-  </si>
-  <si>
     <t>[tmp]/nlp/test_data_04</t>
   </si>
   <si>
@@ -124,16 +70,10 @@
     <t>textract</t>
   </si>
   <si>
-    <t>index</t>
-  </si>
-  <si>
     <t>regex</t>
   </si>
   <si>
     <t>Uber?</t>
-  </si>
-  <si>
-    <t>TIME</t>
   </si>
   <si>
     <t>phrase</t>
@@ -511,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BF5D81-E310-3A45-9ABE-A86114765ABD}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -521,7 +461,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -538,7 +478,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -546,10 +486,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -560,7 +500,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B93662-D338-7A4C-897B-C0C87D585A42}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -572,7 +512,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -589,13 +529,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -603,27 +543,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -634,11 +560,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="C6:E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -649,7 +573,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -665,156 +589,6 @@
       </c>
       <c r="F1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1.2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2.1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>3.1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>3.2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>6.1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -827,7 +601,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -845,7 +621,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -853,23 +629,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>1</v>
@@ -877,7 +653,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -885,7 +661,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>0.2</v>
@@ -893,7 +669,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Add error codes Fix data storage issues Improve tests
</commit_message>
<xml_diff>
--- a/tests/data/test_data_01.xlsx
+++ b/tests/data/test_data_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6392AE28-F5DC-654B-85F2-5C10B79E8EC2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E85FCB-9ECB-F647-B2FF-DE437FC1E5FE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>text</t>
   </si>
@@ -52,16 +52,67 @@
     <t>en_core_web_sm</t>
   </si>
   <si>
+    <t>Uber blew through $1 million a week</t>
+  </si>
+  <si>
+    <t>Android Pay expands to Canada</t>
+  </si>
+  <si>
+    <t>Spotify steps up Asia expansion</t>
+  </si>
+  <si>
+    <t>Google Maps launches location sharing</t>
+  </si>
+  <si>
+    <t>Google rebrands its business apps</t>
+  </si>
+  <si>
+    <t>look what i found on google! 😂</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Google Maps</t>
+  </si>
+  <si>
     <t>PRODUCT</t>
   </si>
   <si>
+    <t>Google</t>
+  </si>
+  <si>
     <t>google</t>
   </si>
   <si>
+    <t>Uber</t>
+  </si>
+  <si>
+    <t>$1 million</t>
+  </si>
+  <si>
+    <t>MONEY</t>
+  </si>
+  <si>
+    <t>Spotify</t>
+  </si>
+  <si>
+    <t>Android Pay</t>
+  </si>
+  <si>
     <t>ORG</t>
   </si>
   <si>
-    <t>[tmp]/nlp/test_data_04</t>
+    <t>GPE</t>
+  </si>
+  <si>
+    <t>0,4</t>
   </si>
   <si>
     <t>Uber blew through $1 million a week. Android Pay expands to Canada. Spotify steps up Asia expansion.</t>
@@ -77,9 +128,6 @@
   </si>
   <si>
     <t>phrase</t>
-  </si>
-  <si>
-    <t>nlp_name</t>
   </si>
   <si>
     <t>nlp_base</t>
@@ -451,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BF5D81-E310-3A45-9ABE-A86114765ABD}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -461,7 +509,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -478,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -486,10 +534,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +560,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -529,13 +577,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -543,13 +591,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -560,9 +608,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -573,7 +621,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -589,6 +637,156 @@
       </c>
       <c r="F1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1.2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2.1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3.1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3.2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>6.1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -599,11 +797,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -621,7 +817,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -629,49 +825,41 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="b">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="1" t="b">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>